<commit_message>
Only violating notes are colored with flag color (except for fill color, which colors whole cantus). Added comment for unfilled leap.
</commit_message>
<xml_diff>
--- a/MGen/notes.xlsx
+++ b/MGen/notes.xlsx
@@ -387,8 +387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55:E60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
CA1: Added new analysis algorithm. It works.
</commit_message>
<xml_diff>
--- a/MGen/notes.xlsx
+++ b/MGen/notes.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
-    <sheet name="Лист1" sheetId="1" r:id="rId2"/>
+    <sheet name="Chrom to dia" sheetId="1" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>C</t>
   </si>
@@ -32,6 +32,9 @@
   <si>
     <t>CC</t>
   </si>
+  <si>
+    <t>Chrom</t>
+  </si>
 </sst>
 </file>
 
@@ -39,7 +42,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0&quot;р.&quot;_-;\-* #,##0&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -82,7 +85,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -387,7 +390,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -418,7 +421,7 @@
         <v>15</v>
       </c>
       <c r="B2">
-        <f>B9+12</f>
+        <f t="shared" ref="B2:B10" si="0">B9+12</f>
         <v>26</v>
       </c>
       <c r="C2">
@@ -446,26 +449,26 @@
         <v>14</v>
       </c>
       <c r="B3">
-        <f>B10+12</f>
+        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C32" si="0">MOD((A3+56), 7)</f>
+        <f t="shared" ref="C3:C32" si="1">MOD((A3+56), 7)</f>
         <v>0</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D32" si="1">ROUNDDOWN(A3/7, 0)*12</f>
+        <f t="shared" ref="D3:D32" si="2">ROUNDDOWN(A3/7, 0)*12</f>
         <v>24</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F32" si="2">E3+D3</f>
+        <f t="shared" ref="F3:F32" si="3">E3+D3</f>
         <v>24</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G32" si="3">F3-B3</f>
+        <f t="shared" ref="G3:G32" si="4">F3-B3</f>
         <v>0</v>
       </c>
     </row>
@@ -474,26 +477,26 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <f>B11+12</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E4">
         <v>11</v>
       </c>
       <c r="F4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="G4">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -502,26 +505,26 @@
         <v>12</v>
       </c>
       <c r="B5">
-        <f>B12+12</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E5">
         <v>9</v>
       </c>
       <c r="F5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="G5">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -530,26 +533,26 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <f>B13+12</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E6">
         <v>7</v>
       </c>
       <c r="F6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="G6">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -558,26 +561,26 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <f>B14+12</f>
+        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E7">
         <v>5</v>
       </c>
       <c r="F7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="G7">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -586,26 +589,26 @@
         <v>9</v>
       </c>
       <c r="B8">
-        <f>B15+12</f>
+        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E8">
         <v>4</v>
       </c>
       <c r="F8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="G8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -614,26 +617,26 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <f>B16+12</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="G9">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -642,26 +645,26 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <f>B17+12</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
       <c r="F10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="G10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -673,22 +676,22 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E11">
         <v>11</v>
       </c>
       <c r="F11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -700,22 +703,22 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E12">
         <v>9</v>
       </c>
       <c r="F12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -727,22 +730,22 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E13">
         <v>7</v>
       </c>
       <c r="F13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -754,22 +757,22 @@
         <v>5</v>
       </c>
       <c r="C14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E14">
         <v>5</v>
       </c>
       <c r="F14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -781,22 +784,22 @@
         <v>4</v>
       </c>
       <c r="C15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E15">
         <v>4</v>
       </c>
       <c r="F15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -808,22 +811,22 @@
         <v>2</v>
       </c>
       <c r="C16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
       <c r="F16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -835,22 +838,22 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
       <c r="F17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -859,26 +862,26 @@
         <v>-1</v>
       </c>
       <c r="B18">
-        <f>B11-12</f>
+        <f t="shared" ref="B18:B32" si="5">B11-12</f>
         <v>-1</v>
       </c>
       <c r="C18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E18">
         <v>11</v>
       </c>
       <c r="F18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="G18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -887,26 +890,26 @@
         <v>-2</v>
       </c>
       <c r="B19">
-        <f>B12-12</f>
+        <f t="shared" si="5"/>
         <v>-3</v>
       </c>
       <c r="C19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E19">
         <v>9</v>
       </c>
       <c r="F19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="G19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -915,26 +918,26 @@
         <v>-3</v>
       </c>
       <c r="B20">
-        <f>B13-12</f>
+        <f t="shared" si="5"/>
         <v>-5</v>
       </c>
       <c r="C20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E20">
         <v>7</v>
       </c>
       <c r="F20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="G20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -943,26 +946,26 @@
         <v>-4</v>
       </c>
       <c r="B21">
-        <f>B14-12</f>
+        <f t="shared" si="5"/>
         <v>-7</v>
       </c>
       <c r="C21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E21">
         <v>5</v>
       </c>
       <c r="F21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5</v>
       </c>
       <c r="G21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -971,26 +974,26 @@
         <v>-5</v>
       </c>
       <c r="B22">
-        <f>B15-12</f>
+        <f t="shared" si="5"/>
         <v>-8</v>
       </c>
       <c r="C22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E22">
         <v>4</v>
       </c>
       <c r="F22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="G22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -999,26 +1002,26 @@
         <v>-6</v>
       </c>
       <c r="B23">
-        <f>B16-12</f>
+        <f t="shared" si="5"/>
         <v>-10</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E23">
         <v>2</v>
       </c>
       <c r="F23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="G23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1027,26 +1030,26 @@
         <v>-7</v>
       </c>
       <c r="B24">
-        <f>B17-12</f>
+        <f t="shared" si="5"/>
         <v>-12</v>
       </c>
       <c r="C24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
       <c r="F24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-12</v>
       </c>
       <c r="G24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1055,26 +1058,26 @@
         <v>-8</v>
       </c>
       <c r="B25">
-        <f>B18-12</f>
+        <f t="shared" si="5"/>
         <v>-13</v>
       </c>
       <c r="C25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E25">
         <v>11</v>
       </c>
       <c r="F25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-1</v>
       </c>
       <c r="G25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1083,26 +1086,26 @@
         <v>-9</v>
       </c>
       <c r="B26">
-        <f>B19-12</f>
+        <f t="shared" si="5"/>
         <v>-15</v>
       </c>
       <c r="C26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="D26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E26">
         <v>9</v>
       </c>
       <c r="F26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-3</v>
       </c>
       <c r="G26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1111,26 +1114,26 @@
         <v>-10</v>
       </c>
       <c r="B27">
-        <f>B20-12</f>
+        <f t="shared" si="5"/>
         <v>-17</v>
       </c>
       <c r="C27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="D27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E27">
         <v>7</v>
       </c>
       <c r="F27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-5</v>
       </c>
       <c r="G27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1139,26 +1142,26 @@
         <v>-11</v>
       </c>
       <c r="B28">
-        <f>B21-12</f>
+        <f t="shared" si="5"/>
         <v>-19</v>
       </c>
       <c r="C28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="D28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E28">
         <v>5</v>
       </c>
       <c r="F28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-7</v>
       </c>
       <c r="G28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1167,26 +1170,26 @@
         <v>-12</v>
       </c>
       <c r="B29">
-        <f>B22-12</f>
+        <f t="shared" si="5"/>
         <v>-20</v>
       </c>
       <c r="C29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="D29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E29">
         <v>4</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-8</v>
       </c>
       <c r="G29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1195,26 +1198,26 @@
         <v>-13</v>
       </c>
       <c r="B30">
-        <f>B23-12</f>
+        <f t="shared" si="5"/>
         <v>-22</v>
       </c>
       <c r="C30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="D30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-12</v>
       </c>
       <c r="E30">
         <v>2</v>
       </c>
       <c r="F30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-10</v>
       </c>
       <c r="G30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1223,26 +1226,26 @@
         <v>-14</v>
       </c>
       <c r="B31">
-        <f>B24-12</f>
+        <f t="shared" si="5"/>
         <v>-24</v>
       </c>
       <c r="C31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="D31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="E31">
         <v>0</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-24</v>
       </c>
       <c r="G31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
@@ -1251,26 +1254,26 @@
         <v>-15</v>
       </c>
       <c r="B32">
-        <f>B25-12</f>
+        <f t="shared" si="5"/>
         <v>-25</v>
       </c>
       <c r="C32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="D32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>-24</v>
       </c>
       <c r="E32">
         <v>11</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>-13</v>
       </c>
       <c r="G32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
@@ -1279,26 +1282,26 @@
         <v>-16</v>
       </c>
       <c r="B33">
-        <f t="shared" ref="B33:B54" si="4">B26-12</f>
+        <f t="shared" ref="B33:B54" si="6">B26-12</f>
         <v>-27</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:C54" si="5">MOD((A33+56), 7)</f>
+        <f t="shared" ref="C33:C54" si="7">MOD((A33+56), 7)</f>
         <v>5</v>
       </c>
       <c r="D33">
-        <f t="shared" ref="D33:D54" si="6">ROUNDDOWN(A33/7, 0)*12</f>
+        <f t="shared" ref="D33:D54" si="8">ROUNDDOWN(A33/7, 0)*12</f>
         <v>-24</v>
       </c>
       <c r="E33">
         <v>9</v>
       </c>
       <c r="F33">
-        <f t="shared" ref="F33:F54" si="7">E33+D33</f>
+        <f t="shared" ref="F33:F54" si="9">E33+D33</f>
         <v>-15</v>
       </c>
       <c r="G33">
-        <f t="shared" ref="G33:G54" si="8">F33-B33</f>
+        <f t="shared" ref="G33:G54" si="10">F33-B33</f>
         <v>12</v>
       </c>
     </row>
@@ -1307,26 +1310,26 @@
         <v>-17</v>
       </c>
       <c r="B34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-29</v>
       </c>
       <c r="C34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-24</v>
       </c>
       <c r="E34">
         <v>7</v>
       </c>
       <c r="F34">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-17</v>
       </c>
       <c r="G34">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1335,26 +1338,26 @@
         <v>-18</v>
       </c>
       <c r="B35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-31</v>
       </c>
       <c r="C35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="D35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-24</v>
       </c>
       <c r="E35">
         <v>5</v>
       </c>
       <c r="F35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-19</v>
       </c>
       <c r="G35">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1363,26 +1366,26 @@
         <v>-19</v>
       </c>
       <c r="B36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-32</v>
       </c>
       <c r="C36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="D36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-24</v>
       </c>
       <c r="E36">
         <v>4</v>
       </c>
       <c r="F36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-20</v>
       </c>
       <c r="G36">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1391,26 +1394,26 @@
         <v>-20</v>
       </c>
       <c r="B37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-34</v>
       </c>
       <c r="C37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="D37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-24</v>
       </c>
       <c r="E37">
         <v>2</v>
       </c>
       <c r="F37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-22</v>
       </c>
       <c r="G37">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1419,26 +1422,26 @@
         <v>-21</v>
       </c>
       <c r="B38">
-        <f t="shared" si="4"/>
-        <v>-36</v>
-      </c>
-      <c r="C38">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D38">
         <f t="shared" si="6"/>
         <v>-36</v>
       </c>
+      <c r="C38">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="8"/>
+        <v>-36</v>
+      </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-36</v>
       </c>
       <c r="G38">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -1447,26 +1450,26 @@
         <v>-22</v>
       </c>
       <c r="B39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-37</v>
       </c>
       <c r="C39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="D39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-36</v>
       </c>
       <c r="E39">
         <v>11</v>
       </c>
       <c r="F39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-25</v>
       </c>
       <c r="G39">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1475,26 +1478,26 @@
         <v>-23</v>
       </c>
       <c r="B40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-39</v>
       </c>
       <c r="C40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-36</v>
       </c>
       <c r="E40">
         <v>9</v>
       </c>
       <c r="F40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-27</v>
       </c>
       <c r="G40">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1503,26 +1506,26 @@
         <v>-24</v>
       </c>
       <c r="B41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-41</v>
       </c>
       <c r="C41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-36</v>
       </c>
       <c r="E41">
         <v>7</v>
       </c>
       <c r="F41">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-29</v>
       </c>
       <c r="G41">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1531,26 +1534,26 @@
         <v>-25</v>
       </c>
       <c r="B42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-43</v>
       </c>
       <c r="C42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="D42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-36</v>
       </c>
       <c r="E42">
         <v>5</v>
       </c>
       <c r="F42">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-31</v>
       </c>
       <c r="G42">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1559,26 +1562,26 @@
         <v>-26</v>
       </c>
       <c r="B43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-44</v>
       </c>
       <c r="C43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="D43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-36</v>
       </c>
       <c r="E43">
         <v>4</v>
       </c>
       <c r="F43">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-32</v>
       </c>
       <c r="G43">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1587,26 +1590,26 @@
         <v>-27</v>
       </c>
       <c r="B44">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-46</v>
       </c>
       <c r="C44">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="D44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-36</v>
       </c>
       <c r="E44">
         <v>2</v>
       </c>
       <c r="F44">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-34</v>
       </c>
       <c r="G44">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1615,26 +1618,26 @@
         <v>-28</v>
       </c>
       <c r="B45">
-        <f t="shared" si="4"/>
-        <v>-48</v>
-      </c>
-      <c r="C45">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D45">
         <f t="shared" si="6"/>
         <v>-48</v>
       </c>
+      <c r="C45">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="8"/>
+        <v>-48</v>
+      </c>
       <c r="E45">
         <v>0</v>
       </c>
       <c r="F45">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-48</v>
       </c>
       <c r="G45">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -1643,26 +1646,26 @@
         <v>-29</v>
       </c>
       <c r="B46">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-49</v>
       </c>
       <c r="C46">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="D46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-48</v>
       </c>
       <c r="E46">
         <v>11</v>
       </c>
       <c r="F46">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-37</v>
       </c>
       <c r="G46">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1671,26 +1674,26 @@
         <v>-30</v>
       </c>
       <c r="B47">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-51</v>
       </c>
       <c r="C47">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-48</v>
       </c>
       <c r="E47">
         <v>9</v>
       </c>
       <c r="F47">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-39</v>
       </c>
       <c r="G47">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1699,26 +1702,26 @@
         <v>-31</v>
       </c>
       <c r="B48">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-53</v>
       </c>
       <c r="C48">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="D48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-48</v>
       </c>
       <c r="E48">
         <v>7</v>
       </c>
       <c r="F48">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-41</v>
       </c>
       <c r="G48">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1727,26 +1730,26 @@
         <v>-32</v>
       </c>
       <c r="B49">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-55</v>
       </c>
       <c r="C49">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="D49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-48</v>
       </c>
       <c r="E49">
         <v>5</v>
       </c>
       <c r="F49">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-43</v>
       </c>
       <c r="G49">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1755,26 +1758,26 @@
         <v>-33</v>
       </c>
       <c r="B50">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-56</v>
       </c>
       <c r="C50">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="D50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-48</v>
       </c>
       <c r="E50">
         <v>4</v>
       </c>
       <c r="F50">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-44</v>
       </c>
       <c r="G50">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1783,26 +1786,26 @@
         <v>-34</v>
       </c>
       <c r="B51">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-58</v>
       </c>
       <c r="C51">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="D51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-48</v>
       </c>
       <c r="E51">
         <v>2</v>
       </c>
       <c r="F51">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-46</v>
       </c>
       <c r="G51">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1811,26 +1814,26 @@
         <v>-35</v>
       </c>
       <c r="B52">
-        <f t="shared" si="4"/>
-        <v>-60</v>
-      </c>
-      <c r="C52">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="D52">
         <f t="shared" si="6"/>
         <v>-60</v>
       </c>
+      <c r="C52">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="8"/>
+        <v>-60</v>
+      </c>
       <c r="E52">
         <v>0</v>
       </c>
       <c r="F52">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-60</v>
       </c>
       <c r="G52">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
@@ -1839,26 +1842,26 @@
         <v>-36</v>
       </c>
       <c r="B53">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-61</v>
       </c>
       <c r="C53">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>6</v>
       </c>
       <c r="D53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-60</v>
       </c>
       <c r="E53">
         <v>11</v>
       </c>
       <c r="F53">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-49</v>
       </c>
       <c r="G53">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1867,26 +1870,26 @@
         <v>-37</v>
       </c>
       <c r="B54">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>-63</v>
       </c>
       <c r="C54">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>5</v>
       </c>
       <c r="D54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>-60</v>
       </c>
       <c r="E54">
         <v>9</v>
       </c>
       <c r="F54">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-51</v>
       </c>
       <c r="G54">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>12</v>
       </c>
     </row>
@@ -1897,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D16"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1908,8 +1911,216 @@
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>72</v>
+      </c>
       <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
SendMIDI: allowed to send NoteON of last note and not send it on next run due to midi_sent_t
</commit_message>
<xml_diff>
--- a/MGen/notes.xlsx
+++ b/MGen/notes.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>C</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Chrom</t>
+  </si>
+  <si>
+    <t>cc % 12</t>
   </si>
 </sst>
 </file>
@@ -83,9 +86,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Денежный" xfId="1" builtinId="4"/>
@@ -1903,11 +1907,12 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="6.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1915,211 +1920,378 @@
       <c r="A1" t="s">
         <v>5</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>86</v>
       </c>
+      <c r="B2">
+        <f>MOD(A2, 12)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>85</v>
       </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B42" si="0">MOD(A3, 12)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>84</v>
       </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>83</v>
       </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>82</v>
       </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>81</v>
       </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>80</v>
       </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>79</v>
       </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>78</v>
       </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>77</v>
       </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>76</v>
       </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>75</v>
       </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>74</v>
       </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>73</v>
       </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>72</v>
       </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>71</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>70</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>69</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>67</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>66</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>64</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>63</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>62</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>61</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>60</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>59</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>57</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>56</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>54</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>53</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>52</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>50</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>49</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>48</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>47</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>46</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AdaptLongBell: Long notes at the beginning and end of phrases have their dynamics smoothed.
</commit_message>
<xml_diff>
--- a/MGen/notes.xlsx
+++ b/MGen/notes.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="84" windowWidth="22980" windowHeight="8484" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="2" r:id="rId1"/>
@@ -1906,8 +1906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2301,12 +2301,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="E19:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <f>40/3</f>
+        <v>13.333333333333334</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <f>80 + 40 - E19</f>
+        <v>106.66666666666667</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>